<commit_message>
fix for the multi min dist and priority strategy
</commit_message>
<xml_diff>
--- a/doc/Benchmarks_stgcenter.xlsx
+++ b/doc/Benchmarks_stgcenter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Desktop\Studium\MoSc_SWT\OSMFirefighter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Desktop\Studium\MoSc_SWT\OSMFirefighter\OSM-Firefighter\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E196CB-E973-45EE-8B7B-4E2B22A770C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ED61D1-B570-43F3-A1A7-ABEA7A6AF8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,17 +79,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,20 +96,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -173,12 +161,173 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -187,15 +336,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,7 +641,7 @@
       <pane xSplit="19" ySplit="5" topLeftCell="T6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,51 +656,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="P1" s="1" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="P1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="P2" s="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="P2" s="12">
         <v>1</v>
       </c>
       <c r="Q2" s="1">
@@ -548,26 +709,26 @@
       <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="P3" s="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="P3" s="12">
         <v>2</v>
       </c>
       <c r="Q3" s="1">
@@ -576,12 +737,12 @@
       <c r="R3" s="1">
         <v>1</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -602,10 +763,10 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="12">
         <v>3</v>
       </c>
       <c r="Q4" s="1">
@@ -614,12 +775,12 @@
       <c r="R4" s="1">
         <v>2</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -656,22 +817,22 @@
       <c r="M5" s="5">
         <v>4</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="P5" s="7">
+      <c r="N5" s="20"/>
+      <c r="P5" s="13">
         <v>4</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="10">
         <v>5</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="10">
         <v>1</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -710,12 +871,12 @@
       <c r="M6" s="6">
         <v>997.7</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="21">
         <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -754,32 +915,56 @@
       <c r="M7" s="6">
         <v>370.1</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="21">
         <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="9"/>
-      <c r="N8">
+      <c r="B8" s="7">
+        <v>33.1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="D8" s="7">
+        <v>19.8</v>
+      </c>
+      <c r="E8" s="6">
+        <v>712.4</v>
+      </c>
+      <c r="F8" s="7">
+        <v>14.9</v>
+      </c>
+      <c r="G8" s="7">
+        <v>44.2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>22.8</v>
+      </c>
+      <c r="I8" s="6">
+        <v>100.7</v>
+      </c>
+      <c r="J8">
+        <v>157.19999999999999</v>
+      </c>
+      <c r="K8">
+        <v>477.9</v>
+      </c>
+      <c r="L8">
+        <v>115.4</v>
+      </c>
+      <c r="M8" s="24">
+        <v>1111.5999999999999</v>
+      </c>
+      <c r="N8" s="21">
         <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="7">
@@ -818,39 +1003,95 @@
       <c r="M9" s="6">
         <v>322.2</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="21">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="9"/>
-      <c r="N10">
+      <c r="B10" s="7">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="C10" s="7">
+        <v>212.7</v>
+      </c>
+      <c r="D10" s="7">
+        <v>36.9</v>
+      </c>
+      <c r="E10" s="6">
+        <v>729.9</v>
+      </c>
+      <c r="F10" s="7">
+        <v>25.7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>63.4</v>
+      </c>
+      <c r="H10" s="7">
+        <v>49.4</v>
+      </c>
+      <c r="I10" s="6">
+        <v>103.1</v>
+      </c>
+      <c r="J10">
+        <v>284</v>
+      </c>
+      <c r="K10">
+        <v>697.4</v>
+      </c>
+      <c r="L10">
+        <v>253.4</v>
+      </c>
+      <c r="M10" s="24">
+        <v>1142.5999999999999</v>
+      </c>
+      <c r="N10" s="21">
         <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11">
+      <c r="B11" s="17">
+        <v>24.9</v>
+      </c>
+      <c r="C11" s="17">
+        <v>111.7</v>
+      </c>
+      <c r="D11" s="17">
+        <v>15.7</v>
+      </c>
+      <c r="E11" s="18">
+        <v>592.4</v>
+      </c>
+      <c r="F11" s="17">
+        <v>12.2</v>
+      </c>
+      <c r="G11" s="17">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="H11" s="17">
+        <v>17.7</v>
+      </c>
+      <c r="I11" s="18">
+        <v>94.7</v>
+      </c>
+      <c r="J11" s="17">
+        <v>127.1</v>
+      </c>
+      <c r="K11" s="17">
+        <v>386.9</v>
+      </c>
+      <c r="L11" s="17">
+        <v>89.4</v>
+      </c>
+      <c r="M11" s="18">
+        <v>1025.0999999999999</v>
+      </c>
+      <c r="N11" s="22">
         <v>1000</v>
       </c>
       <c r="S11" s="1"/>

</xml_diff>